<commit_message>
Added, time incrementation, border fixes, title and scripture changes
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[h]:mm"/>
+    <numFmt numFmtId="165" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="[hh]:mm"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <name val="Calibri"/>
@@ -94,12 +98,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -116,11 +135,25 @@
         <color rgb="00FFFFFF"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00FFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="00FFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="00FFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00808080"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -148,42 +181,61 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:D999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -572,1955 +624,2377 @@
     <col width="11.85546875" customWidth="1" style="2" min="1" max="1"/>
     <col width="16.7109375" customWidth="1" style="2" min="2" max="2"/>
     <col width="58.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9.140625" customWidth="1" style="2" min="4" max="4"/>
+    <col width="9.140625" customWidth="1" style="11" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1">
-      <c r="A1" s="12" t="n"/>
-      <c r="B1" s="12" t="n"/>
-      <c r="C1" s="13" t="inlineStr">
-        <is>
-          <t>[MONTH] [YEAR] Our Christian Life &amp; Ministry</t>
-        </is>
-      </c>
-      <c r="D1" s="12" t="n"/>
+      <c r="A1" s="15" t="n"/>
+      <c r="B1" s="16" t="inlineStr">
+        <is>
+          <t>Life and Ministry Meeting Workbook, January 2023</t>
+        </is>
+      </c>
+      <c r="C1" s="15" t="n"/>
+      <c r="D1" s="15" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B2" s="15" t="inlineStr">
+      <c r="A2" s="17" t="inlineStr">
+        <is>
+          <t>Week 1</t>
+        </is>
+      </c>
+      <c r="B2" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C2" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D2" s="14" t="inlineStr">
+      <c r="C2" s="19" t="inlineStr">
+        <is>
+          <t>2 KINGS 22-23</t>
+        </is>
+      </c>
+      <c r="D2" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="21" t="inlineStr">
         <is>
           <t>Song 28</t>
         </is>
       </c>
-      <c r="B3" s="12" t="n"/>
-      <c r="C3" s="18" t="inlineStr">
+      <c r="B3" s="15" t="n"/>
+      <c r="C3" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D3" s="19" t="inlineStr">
+      <c r="D3" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="n"/>
-      <c r="B4" s="12" t="n"/>
-      <c r="C4" s="12" t="n"/>
-      <c r="D4" s="20" t="n">
+      <c r="A4" s="15" t="n"/>
+      <c r="B4" s="15" t="n"/>
+      <c r="C4" s="15" t="n"/>
+      <c r="D4" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="n"/>
-      <c r="B5" s="12" t="n"/>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="A5" s="15" t="n"/>
+      <c r="B5" s="15" t="n"/>
+      <c r="C5" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D5" s="12" t="n"/>
+      <c r="D5" s="15" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="inlineStr">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B6" s="12" t="n"/>
-      <c r="C6" s="22" t="inlineStr">
+      <c r="B6" s="26" t="n"/>
+      <c r="C6" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D6" s="12" t="n"/>
+      <c r="D6" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="inlineStr">
+      <c r="A7" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B7" s="12" t="n"/>
-      <c r="C7" s="22" t="inlineStr">
+      <c r="B7" s="26" t="n"/>
+      <c r="C7" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Why Be Humble?”: 
 </t>
         </is>
       </c>
-      <c r="D7" s="12" t="n"/>
+      <c r="D7" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="inlineStr">
+      <c r="A8" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B8" s="12" t="n"/>
-      <c r="C8" s="22" t="inlineStr">
+      <c r="B8" s="26" t="n"/>
+      <c r="C8" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D8" s="12" t="n"/>
+      <c r="D8" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="inlineStr">
+      <c r="A9" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B9" s="12" t="n"/>
-      <c r="C9" s="22" t="inlineStr">
+      <c r="B9" s="26" t="n"/>
+      <c r="C9" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 23:16-25 (th study 2)
 </t>
         </is>
       </c>
-      <c r="D9" s="12" t="n"/>
+      <c r="D9" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="n"/>
-      <c r="B10" s="12" t="n"/>
-      <c r="C10" s="12" t="inlineStr"/>
-      <c r="D10" s="12" t="n"/>
+      <c r="A10" s="15" t="n"/>
+      <c r="B10" s="15" t="n"/>
+      <c r="C10" s="15" t="inlineStr"/>
+      <c r="D10" s="15" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="n"/>
-      <c r="B11" s="12" t="n"/>
-      <c r="C11" s="23" t="inlineStr">
+      <c r="A11" s="15" t="n"/>
+      <c r="B11" s="15" t="n"/>
+      <c r="C11" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D11" s="12" t="n"/>
+      <c r="D11" s="15" t="n"/>
     </row>
     <row r="12" ht="21" customHeight="1">
-      <c r="A12" s="19" t="inlineStr">
+      <c r="A12" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B12" s="12" t="n"/>
-      <c r="C12" s="22" t="inlineStr">
+      <c r="B12" s="26" t="n"/>
+      <c r="C12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call Video:  Discussion. Play the video Initial Call: Prayer —Ps 65:2. Stop the video at each pause, and ask the audience the questions that appear in the video.
 </t>
         </is>
       </c>
-      <c r="D12" s="12" t="n"/>
+      <c r="D12" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="19" t="inlineStr">
+      <c r="A13" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B13" s="12" t="n"/>
-      <c r="C13" s="22" t="inlineStr">
+      <c r="B13" s="26" t="n"/>
+      <c r="C13" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. (th study 1)
 </t>
         </is>
       </c>
-      <c r="D13" s="12" t="n"/>
+      <c r="D13" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="inlineStr">
+      <c r="A14" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B14" s="12" t="n"/>
-      <c r="C14" s="22" t="inlineStr">
+      <c r="B14" s="26" t="n"/>
+      <c r="C14" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 16)
 </t>
         </is>
       </c>
-      <c r="D14" s="12" t="n"/>
+      <c r="D14" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="n"/>
-      <c r="B15" s="12" t="n"/>
-      <c r="C15" s="12" t="inlineStr"/>
-      <c r="D15" s="12" t="n"/>
+      <c r="A15" s="15" t="n"/>
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="15" t="inlineStr"/>
+      <c r="D15" s="15" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="17" t="inlineStr">
+      <c r="A16" s="21" t="inlineStr">
         <is>
           <t>Song 120</t>
         </is>
       </c>
-      <c r="B16" s="12" t="n"/>
-      <c r="C16" s="24" t="inlineStr">
+      <c r="B16" s="15" t="n"/>
+      <c r="C16" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D16" s="12" t="n"/>
+      <c r="D16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="19" t="inlineStr">
+      <c r="A17" s="25" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B17" s="12" t="n"/>
-      <c r="C17" s="22" t="inlineStr">
+      <c r="B17" s="26" t="n"/>
+      <c r="C17" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Humble or Haughty? (Jas 4:6):  Discussion. Play the video. Then ask the audience: What is the difference between humility and haughtiness? What can we learn from Moses’ example? Why are you determined to remain humble?
 </t>
         </is>
       </c>
-      <c r="D17" s="12" t="n"/>
+      <c r="D17" s="28" t="n">
+        <v>0.30625</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="19" t="inlineStr">
+      <c r="A18" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B18" s="12" t="n"/>
-      <c r="C18" s="22" t="inlineStr">
+      <c r="B18" s="26" t="n"/>
+      <c r="C18" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 33
 </t>
         </is>
       </c>
-      <c r="D18" s="12" t="n"/>
+      <c r="D18" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="19" t="inlineStr">
+      <c r="A19" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B19" s="12" t="n"/>
-      <c r="C19" s="22" t="inlineStr">
+      <c r="B19" s="26" t="n"/>
+      <c r="C19" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D19" s="12" t="n"/>
+      <c r="D19" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="n"/>
-      <c r="B20" s="12" t="n"/>
-      <c r="C20" s="12" t="inlineStr"/>
-      <c r="D20" s="12" t="n"/>
+      <c r="A20" s="15" t="n"/>
+      <c r="B20" s="15" t="n"/>
+      <c r="C20" s="15" t="inlineStr"/>
+      <c r="D20" s="15" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="17" t="inlineStr">
+      <c r="A21" s="21" t="inlineStr">
         <is>
           <t>Song 23</t>
         </is>
       </c>
-      <c r="B21" s="12" t="n"/>
-      <c r="C21" s="18" t="inlineStr">
+      <c r="B21" s="15" t="n"/>
+      <c r="C21" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D21" s="12" t="n"/>
+      <c r="D21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="n"/>
-      <c r="B22" s="12" t="n"/>
-      <c r="C22" s="13" t="n"/>
-      <c r="D22" s="12" t="n"/>
+      <c r="A22" s="15" t="n"/>
+      <c r="B22" s="15" t="n"/>
+      <c r="C22" s="31" t="n"/>
+      <c r="D22" s="15" t="n"/>
     </row>
     <row r="23" ht="21" customHeight="1">
-      <c r="A23" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B23" s="15" t="inlineStr">
+      <c r="A23" s="17" t="inlineStr">
+        <is>
+          <t>Week 2</t>
+        </is>
+      </c>
+      <c r="B23" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C23" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D23" s="14" t="inlineStr">
+      <c r="C23" s="19" t="inlineStr">
+        <is>
+          <t>2 KINGS 24-25</t>
+        </is>
+      </c>
+      <c r="D23" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="17" t="inlineStr">
+      <c r="A24" s="21" t="inlineStr">
         <is>
           <t>Song 60</t>
         </is>
       </c>
-      <c r="B24" s="12" t="n"/>
-      <c r="C24" s="18" t="inlineStr">
+      <c r="B24" s="15" t="n"/>
+      <c r="C24" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D24" s="19" t="inlineStr">
+      <c r="D24" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="n"/>
-      <c r="B25" s="12" t="n"/>
-      <c r="C25" s="12" t="n"/>
-      <c r="D25" s="20" t="n">
+      <c r="A25" s="15" t="n"/>
+      <c r="B25" s="15" t="n"/>
+      <c r="C25" s="15" t="n"/>
+      <c r="D25" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12" t="n"/>
-      <c r="B26" s="12" t="n"/>
-      <c r="C26" s="21" t="inlineStr">
+      <c r="A26" s="15" t="n"/>
+      <c r="B26" s="15" t="n"/>
+      <c r="C26" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D26" s="12" t="n"/>
+      <c r="D26" s="15" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="19" t="inlineStr">
+      <c r="A27" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B27" s="12" t="n"/>
-      <c r="C27" s="22" t="inlineStr">
+      <c r="B27" s="26" t="n"/>
+      <c r="C27" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D27" s="12" t="n"/>
+      <c r="D27" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="19" t="inlineStr">
+      <c r="A28" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B28" s="12" t="n"/>
-      <c r="C28" s="22" t="inlineStr">
+      <c r="B28" s="26" t="n"/>
+      <c r="C28" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Maintain Your Sense of Urgency”: 
 </t>
         </is>
       </c>
-      <c r="D28" s="12" t="n"/>
+      <c r="D28" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="19" t="inlineStr">
+      <c r="A29" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B29" s="12" t="n"/>
-      <c r="C29" s="22" t="inlineStr">
+      <c r="B29" s="26" t="n"/>
+      <c r="C29" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D29" s="12" t="n"/>
+      <c r="D29" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="19" t="inlineStr">
+      <c r="A30" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B30" s="12" t="n"/>
-      <c r="C30" s="22" t="inlineStr">
+      <c r="B30" s="26" t="n"/>
+      <c r="C30" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  2Ki 24:1-17 (th study 11)
 </t>
         </is>
       </c>
-      <c r="D30" s="12" t="n"/>
+      <c r="D30" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="12" t="n"/>
-      <c r="B31" s="12" t="n"/>
-      <c r="C31" s="12" t="inlineStr"/>
-      <c r="D31" s="12" t="n"/>
+      <c r="A31" s="15" t="n"/>
+      <c r="B31" s="15" t="n"/>
+      <c r="C31" s="15" t="inlineStr"/>
+      <c r="D31" s="15" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="12" t="n"/>
-      <c r="B32" s="12" t="n"/>
-      <c r="C32" s="23" t="inlineStr">
+      <c r="A32" s="15" t="n"/>
+      <c r="B32" s="15" t="n"/>
+      <c r="C32" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D32" s="12" t="n"/>
+      <c r="D32" s="15" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="19" t="inlineStr">
+      <c r="A33" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B33" s="12" t="n"/>
-      <c r="C33" s="22" t="inlineStr">
+      <c r="B33" s="26" t="n"/>
+      <c r="C33" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit Video:  Discussion. Play the video Return Visit: Prayer —1Jo 5:14. Stop the video at each pause, and ask the audience the questions that appear in the video.
 </t>
         </is>
       </c>
-      <c r="D33" s="12" t="n"/>
+      <c r="D33" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
     </row>
     <row r="34" ht="21" customHeight="1">
-      <c r="A34" s="19" t="inlineStr">
+      <c r="A34" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B34" s="12" t="n"/>
-      <c r="C34" s="22" t="inlineStr">
+      <c r="B34" s="26" t="n"/>
+      <c r="C34" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Use the sample conversation topic. (th study 15)
 </t>
         </is>
       </c>
-      <c r="D34" s="12" t="n"/>
+      <c r="D34" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="19" t="inlineStr">
+      <c r="A35" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B35" s="12" t="n"/>
-      <c r="C35" s="22" t="inlineStr">
+      <c r="B35" s="26" t="n"/>
+      <c r="C35" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic, and start a Bible study in lesson 01 of the Enjoy Life Forever! brochure. (th study 19)
 </t>
         </is>
       </c>
-      <c r="D35" s="12" t="n"/>
+      <c r="D35" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="12" t="n"/>
-      <c r="B36" s="12" t="n"/>
-      <c r="C36" s="12" t="inlineStr"/>
-      <c r="D36" s="12" t="n"/>
+      <c r="A36" s="15" t="n"/>
+      <c r="B36" s="15" t="n"/>
+      <c r="C36" s="15" t="inlineStr"/>
+      <c r="D36" s="15" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="17" t="inlineStr">
+      <c r="A37" s="21" t="inlineStr">
         <is>
           <t>Song 143</t>
         </is>
       </c>
-      <c r="B37" s="12" t="n"/>
-      <c r="C37" s="24" t="inlineStr">
+      <c r="B37" s="15" t="n"/>
+      <c r="C37" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D37" s="12" t="n"/>
+      <c r="D37" s="15" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="19" t="inlineStr">
+      <c r="A38" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B38" s="12" t="n"/>
-      <c r="C38" s="22" t="inlineStr">
+      <c r="B38" s="26" t="n"/>
+      <c r="C38" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
 </t>
         </is>
       </c>
-      <c r="D38" s="12" t="n"/>
+      <c r="D38" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="19" t="inlineStr">
+      <c r="A39" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B39" s="12" t="n"/>
-      <c r="C39" s="22" t="inlineStr">
+      <c r="B39" s="26" t="n"/>
+      <c r="C39" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff section 2 review
 </t>
         </is>
       </c>
-      <c r="D39" s="12" t="n"/>
+      <c r="D39" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="19" t="inlineStr">
+      <c r="A40" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B40" s="12" t="n"/>
-      <c r="C40" s="22" t="inlineStr">
+      <c r="B40" s="26" t="n"/>
+      <c r="C40" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D40" s="12" t="n"/>
+      <c r="D40" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="12" t="n"/>
-      <c r="B41" s="12" t="n"/>
-      <c r="C41" s="12" t="inlineStr"/>
-      <c r="D41" s="12" t="n"/>
+      <c r="A41" s="15" t="n"/>
+      <c r="B41" s="15" t="n"/>
+      <c r="C41" s="15" t="inlineStr"/>
+      <c r="D41" s="15" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="17" t="inlineStr">
+      <c r="A42" s="21" t="inlineStr">
         <is>
           <t>Song 54</t>
         </is>
       </c>
-      <c r="B42" s="12" t="n"/>
-      <c r="C42" s="18" t="inlineStr">
+      <c r="B42" s="15" t="n"/>
+      <c r="C42" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D42" s="12" t="n"/>
+      <c r="D42" s="15" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="12" t="n"/>
-      <c r="B43" s="12" t="n"/>
-      <c r="C43" s="13" t="n"/>
-      <c r="D43" s="12" t="n"/>
+      <c r="A43" s="15" t="n"/>
+      <c r="B43" s="15" t="n"/>
+      <c r="C43" s="31" t="n"/>
+      <c r="D43" s="15" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B44" s="15" t="inlineStr">
+      <c r="A44" s="17" t="inlineStr">
+        <is>
+          <t>Week 3</t>
+        </is>
+      </c>
+      <c r="B44" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C44" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D44" s="14" t="inlineStr">
+      <c r="C44" s="19" t="inlineStr">
+        <is>
+          <t>1 CHRONICLES 1-3</t>
+        </is>
+      </c>
+      <c r="D44" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
     <row r="45" ht="21" customHeight="1">
-      <c r="A45" s="17" t="inlineStr">
+      <c r="A45" s="21" t="inlineStr">
         <is>
           <t>Song 96</t>
         </is>
       </c>
-      <c r="B45" s="12" t="n"/>
-      <c r="C45" s="18" t="inlineStr">
+      <c r="B45" s="15" t="n"/>
+      <c r="C45" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D45" s="19" t="inlineStr">
+      <c r="D45" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="12" t="n"/>
-      <c r="B46" s="12" t="n"/>
-      <c r="C46" s="12" t="n"/>
-      <c r="D46" s="20" t="n">
+    <row r="46" ht="21" customHeight="1">
+      <c r="A46" s="15" t="n"/>
+      <c r="B46" s="15" t="n"/>
+      <c r="C46" s="15" t="n"/>
+      <c r="D46" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="12" t="n"/>
-      <c r="B47" s="12" t="n"/>
-      <c r="C47" s="21" t="inlineStr">
+    <row r="47" ht="21" customHeight="1">
+      <c r="A47" s="15" t="n"/>
+      <c r="B47" s="15" t="n"/>
+      <c r="C47" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D47" s="12" t="n"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="19" t="inlineStr">
+      <c r="D47" s="15" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B48" s="12" t="n"/>
-      <c r="C48" s="22" t="inlineStr">
+      <c r="B48" s="26" t="n"/>
+      <c r="C48" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D48" s="12" t="n"/>
+      <c r="D48" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="19" t="inlineStr">
+      <c r="A49" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B49" s="12" t="n"/>
-      <c r="C49" s="22" t="inlineStr">
+      <c r="B49" s="26" t="n"/>
+      <c r="C49" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“The Bible —A Book of Fact, Not Fiction”: 
 </t>
         </is>
       </c>
-      <c r="D49" s="12" t="n"/>
+      <c r="D49" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="19" t="inlineStr">
+      <c r="A50" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B50" s="12" t="n"/>
-      <c r="C50" s="22" t="inlineStr">
+      <c r="B50" s="26" t="n"/>
+      <c r="C50" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D50" s="12" t="n"/>
+      <c r="D50" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="19" t="inlineStr">
+      <c r="A51" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B51" s="12" t="n"/>
-      <c r="C51" s="22" t="inlineStr">
+      <c r="B51" s="26" t="n"/>
+      <c r="C51" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 1:43-54 (th study 5)
 </t>
         </is>
       </c>
-      <c r="D51" s="12" t="n"/>
+      <c r="D51" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="12" t="n"/>
-      <c r="B52" s="12" t="n"/>
-      <c r="C52" s="12" t="inlineStr"/>
-      <c r="D52" s="12" t="n"/>
+      <c r="A52" s="15" t="n"/>
+      <c r="B52" s="15" t="n"/>
+      <c r="C52" s="15" t="inlineStr"/>
+      <c r="D52" s="15" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="12" t="n"/>
-      <c r="B53" s="12" t="n"/>
-      <c r="C53" s="23" t="inlineStr">
+      <c r="A53" s="15" t="n"/>
+      <c r="B53" s="15" t="n"/>
+      <c r="C53" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D53" s="12" t="n"/>
+      <c r="D53" s="15" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="19" t="inlineStr">
+      <c r="A54" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B54" s="12" t="n"/>
-      <c r="C54" s="22" t="inlineStr">
+      <c r="B54" s="26" t="n"/>
+      <c r="C54" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a magazine to address a topic raised by the householder. (th study 4)
 </t>
         </is>
       </c>
-      <c r="D54" s="12" t="n"/>
+      <c r="D54" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="19" t="inlineStr">
+      <c r="A55" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B55" s="12" t="n"/>
-      <c r="C55" s="22" t="inlineStr">
+      <c r="B55" s="26" t="n"/>
+      <c r="C55" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 1)
 </t>
         </is>
       </c>
-      <c r="D55" s="12" t="n"/>
-    </row>
-    <row r="56" ht="21" customHeight="1">
-      <c r="A56" s="19" t="inlineStr">
+      <c r="D55" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B56" s="12" t="n"/>
-      <c r="C56" s="22" t="inlineStr">
+      <c r="B56" s="26" t="n"/>
+      <c r="C56" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 point 7 and Some People Say (th study 8)
 </t>
         </is>
       </c>
-      <c r="D56" s="12" t="n"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="12" t="n"/>
-      <c r="B57" s="12" t="n"/>
-      <c r="C57" s="12" t="inlineStr"/>
-      <c r="D57" s="12" t="n"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="17" t="inlineStr">
+      <c r="D56" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="15" t="n"/>
+      <c r="B57" s="15" t="n"/>
+      <c r="C57" s="15" t="inlineStr"/>
+      <c r="D57" s="15" t="n"/>
+    </row>
+    <row r="58" ht="21" customHeight="1">
+      <c r="A58" s="21" t="inlineStr">
         <is>
           <t>Song 98</t>
         </is>
       </c>
-      <c r="B58" s="12" t="n"/>
-      <c r="C58" s="24" t="inlineStr">
+      <c r="B58" s="15" t="n"/>
+      <c r="C58" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D58" s="12" t="n"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="19" t="inlineStr">
+      <c r="D58" s="15" t="n"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="25" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B59" s="12" t="n"/>
-      <c r="C59" s="22" t="inlineStr">
+      <c r="B59" s="26" t="n"/>
+      <c r="C59" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Faith in God’s Word”:  Discussion and video.
 </t>
         </is>
       </c>
-      <c r="D59" s="12" t="n"/>
+      <c r="D59" s="28" t="n">
+        <v>0.30625</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="19" t="inlineStr">
+      <c r="A60" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B60" s="12" t="n"/>
-      <c r="C60" s="22" t="inlineStr">
+      <c r="B60" s="26" t="n"/>
+      <c r="C60" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 34
 </t>
         </is>
       </c>
-      <c r="D60" s="12" t="n"/>
+      <c r="D60" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="19" t="inlineStr">
+      <c r="A61" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B61" s="12" t="n"/>
-      <c r="C61" s="22" t="inlineStr">
+      <c r="B61" s="26" t="n"/>
+      <c r="C61" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D61" s="12" t="n"/>
+      <c r="D61" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="12" t="n"/>
-      <c r="B62" s="12" t="n"/>
-      <c r="C62" s="12" t="inlineStr"/>
-      <c r="D62" s="12" t="n"/>
+      <c r="A62" s="15" t="n"/>
+      <c r="B62" s="15" t="n"/>
+      <c r="C62" s="15" t="inlineStr"/>
+      <c r="D62" s="15" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="17" t="inlineStr">
+      <c r="A63" s="21" t="inlineStr">
         <is>
           <t>Song 89</t>
         </is>
       </c>
-      <c r="B63" s="12" t="n"/>
-      <c r="C63" s="18" t="inlineStr">
+      <c r="B63" s="15" t="n"/>
+      <c r="C63" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D63" s="12" t="n"/>
+      <c r="D63" s="15" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="12" t="n"/>
-      <c r="B64" s="12" t="n"/>
-      <c r="C64" s="13" t="n"/>
-      <c r="D64" s="12" t="n"/>
+      <c r="A64" s="15" t="n"/>
+      <c r="B64" s="15" t="n"/>
+      <c r="C64" s="31" t="n"/>
+      <c r="D64" s="15" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B65" s="15" t="inlineStr">
+      <c r="A65" s="17" t="inlineStr">
+        <is>
+          <t>Week 4</t>
+        </is>
+      </c>
+      <c r="B65" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C65" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D65" s="14" t="inlineStr">
+      <c r="C65" s="19" t="inlineStr">
+        <is>
+          <t>1 CHRONICLES 4-6</t>
+        </is>
+      </c>
+      <c r="D65" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="17" t="inlineStr">
+      <c r="A66" s="21" t="inlineStr">
         <is>
           <t>Song 42</t>
         </is>
       </c>
-      <c r="B66" s="12" t="n"/>
-      <c r="C66" s="18" t="inlineStr">
+      <c r="B66" s="15" t="n"/>
+      <c r="C66" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D66" s="19" t="inlineStr">
+      <c r="D66" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
-    <row r="67" ht="21" customHeight="1">
-      <c r="A67" s="12" t="n"/>
-      <c r="B67" s="12" t="n"/>
-      <c r="C67" s="12" t="n"/>
-      <c r="D67" s="20" t="n">
+    <row r="67">
+      <c r="A67" s="15" t="n"/>
+      <c r="B67" s="15" t="n"/>
+      <c r="C67" s="15" t="n"/>
+      <c r="D67" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="12" t="n"/>
-      <c r="B68" s="12" t="n"/>
-      <c r="C68" s="21" t="inlineStr">
+    <row r="68">
+      <c r="A68" s="15" t="n"/>
+      <c r="B68" s="15" t="n"/>
+      <c r="C68" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D68" s="12" t="n"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="19" t="inlineStr">
+      <c r="D68" s="15" t="n"/>
+    </row>
+    <row r="69" ht="21" customHeight="1">
+      <c r="A69" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B69" s="12" t="n"/>
-      <c r="C69" s="22" t="inlineStr">
+      <c r="B69" s="26" t="n"/>
+      <c r="C69" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D69" s="12" t="n"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="19" t="inlineStr">
+      <c r="D69" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B70" s="12" t="n"/>
-      <c r="C70" s="22" t="inlineStr">
+      <c r="B70" s="26" t="n"/>
+      <c r="C70" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“What Do My Prayers Reveal About Me?”: 
 </t>
         </is>
       </c>
-      <c r="D70" s="12" t="n"/>
+      <c r="D70" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="19" t="inlineStr">
+      <c r="A71" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B71" s="12" t="n"/>
-      <c r="C71" s="22" t="inlineStr">
+      <c r="B71" s="26" t="n"/>
+      <c r="C71" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D71" s="12" t="n"/>
+      <c r="D71" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="19" t="inlineStr">
+      <c r="A72" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B72" s="12" t="n"/>
-      <c r="C72" s="22" t="inlineStr">
+      <c r="B72" s="26" t="n"/>
+      <c r="C72" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 6:61-81 (th study 2)
 </t>
         </is>
       </c>
-      <c r="D72" s="12" t="n"/>
+      <c r="D72" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" s="12" t="n"/>
-      <c r="B73" s="12" t="n"/>
-      <c r="C73" s="12" t="inlineStr"/>
-      <c r="D73" s="12" t="n"/>
+      <c r="A73" s="15" t="n"/>
+      <c r="B73" s="15" t="n"/>
+      <c r="C73" s="15" t="inlineStr"/>
+      <c r="D73" s="15" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="12" t="n"/>
-      <c r="B74" s="12" t="n"/>
-      <c r="C74" s="23" t="inlineStr">
+      <c r="A74" s="15" t="n"/>
+      <c r="B74" s="15" t="n"/>
+      <c r="C74" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D74" s="12" t="n"/>
+      <c r="D74" s="15" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" s="19" t="inlineStr">
+      <c r="A75" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B75" s="12" t="n"/>
-      <c r="C75" s="22" t="inlineStr">
+      <c r="B75" s="26" t="n"/>
+      <c r="C75" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Use the sample conversation topic. Respond to a common objection. (th study 3)
 </t>
         </is>
       </c>
-      <c r="D75" s="12" t="n"/>
+      <c r="D75" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" s="19" t="inlineStr">
+      <c r="A76" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B76" s="12" t="n"/>
-      <c r="C76" s="22" t="inlineStr">
+      <c r="B76" s="26" t="n"/>
+      <c r="C76" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Why Study the Bible? (th study 14)
 </t>
         </is>
       </c>
-      <c r="D76" s="12" t="n"/>
+      <c r="D76" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" s="19" t="inlineStr">
+      <c r="A77" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B77" s="12" t="n"/>
-      <c r="C77" s="22" t="inlineStr">
+      <c r="B77" s="26" t="n"/>
+      <c r="C77" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 08 summary, review, and goal (th study 9)
 </t>
         </is>
       </c>
-      <c r="D77" s="12" t="n"/>
+      <c r="D77" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" s="12" t="n"/>
-      <c r="B78" s="12" t="n"/>
-      <c r="C78" s="12" t="inlineStr"/>
-      <c r="D78" s="12" t="n"/>
+      <c r="A78" s="15" t="n"/>
+      <c r="B78" s="15" t="n"/>
+      <c r="C78" s="15" t="inlineStr"/>
+      <c r="D78" s="15" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" s="17" t="inlineStr">
+      <c r="A79" s="21" t="inlineStr">
         <is>
           <t>Song 127</t>
         </is>
       </c>
-      <c r="B79" s="12" t="n"/>
-      <c r="C79" s="24" t="inlineStr">
+      <c r="B79" s="15" t="n"/>
+      <c r="C79" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D79" s="12" t="n"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="19" t="inlineStr">
+      <c r="D79" s="15" t="n"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="25" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B80" s="12" t="n"/>
-      <c r="C80" s="22" t="inlineStr">
+      <c r="B80" s="26" t="n"/>
+      <c r="C80" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Prepare Now for a Medical Emergency”:  Discussion and video. To be handled by an elder. Allow time for several comments after the video.
 </t>
         </is>
       </c>
-      <c r="D80" s="12" t="n"/>
+      <c r="D80" s="28" t="n">
+        <v>0.30625</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" s="19" t="inlineStr">
+      <c r="A81" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B81" s="12" t="n"/>
-      <c r="C81" s="22" t="inlineStr">
+      <c r="B81" s="26" t="n"/>
+      <c r="C81" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 35
 </t>
         </is>
       </c>
-      <c r="D81" s="12" t="n"/>
+      <c r="D81" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" s="19" t="inlineStr">
+      <c r="A82" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B82" s="12" t="n"/>
-      <c r="C82" s="22" t="inlineStr">
+      <c r="B82" s="26" t="n"/>
+      <c r="C82" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D82" s="12" t="n"/>
+      <c r="D82" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="12" t="n"/>
-      <c r="B83" s="12" t="n"/>
-      <c r="C83" s="12" t="inlineStr"/>
-      <c r="D83" s="12" t="n"/>
+      <c r="A83" s="15" t="n"/>
+      <c r="B83" s="15" t="n"/>
+      <c r="C83" s="15" t="inlineStr"/>
+      <c r="D83" s="15" t="n"/>
     </row>
     <row r="84">
-      <c r="A84" s="17" t="inlineStr">
+      <c r="A84" s="21" t="inlineStr">
         <is>
           <t>Song 88</t>
         </is>
       </c>
-      <c r="B84" s="12" t="n"/>
-      <c r="C84" s="18" t="inlineStr">
+      <c r="B84" s="15" t="n"/>
+      <c r="C84" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D84" s="12" t="n"/>
+      <c r="D84" s="15" t="n"/>
     </row>
     <row r="85">
-      <c r="A85" s="12" t="n"/>
-      <c r="B85" s="12" t="n"/>
-      <c r="C85" s="13" t="n"/>
-      <c r="D85" s="12" t="n"/>
+      <c r="A85" s="15" t="n"/>
+      <c r="B85" s="15" t="n"/>
+      <c r="C85" s="31" t="n"/>
+      <c r="D85" s="15" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B86" s="15" t="inlineStr">
+      <c r="A86" s="15" t="n"/>
+      <c r="B86" s="15" t="n"/>
+      <c r="C86" s="31" t="n"/>
+      <c r="D86" s="15" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="15" t="n"/>
+      <c r="B87" s="16" t="inlineStr">
+        <is>
+          <t>Life and Ministry Meeting Workbook, February 2023</t>
+        </is>
+      </c>
+      <c r="C87" s="15" t="n"/>
+      <c r="D87" s="15" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="17" t="inlineStr">
+        <is>
+          <t>Week 1</t>
+        </is>
+      </c>
+      <c r="B88" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C86" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D86" s="14" t="inlineStr">
+      <c r="C88" s="19" t="inlineStr">
+        <is>
+          <t>1 CHRONICLES 7-9</t>
+        </is>
+      </c>
+      <c r="D88" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="17" t="inlineStr">
+    <row r="89">
+      <c r="A89" s="21" t="inlineStr">
         <is>
           <t>Song 84</t>
         </is>
       </c>
-      <c r="B87" s="12" t="n"/>
-      <c r="C87" s="18" t="inlineStr">
+      <c r="B89" s="15" t="n"/>
+      <c r="C89" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D87" s="19" t="inlineStr">
+      <c r="D89" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="12" t="n"/>
-      <c r="B88" s="12" t="n"/>
-      <c r="C88" s="12" t="n"/>
-      <c r="D88" s="20" t="n">
+    <row r="90">
+      <c r="A90" s="15" t="n"/>
+      <c r="B90" s="15" t="n"/>
+      <c r="C90" s="15" t="n"/>
+      <c r="D90" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="12" t="n"/>
-      <c r="B89" s="12" t="n"/>
-      <c r="C89" s="21" t="inlineStr">
+    <row r="91">
+      <c r="A91" s="15" t="n"/>
+      <c r="B91" s="15" t="n"/>
+      <c r="C91" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D89" s="12" t="n"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="19" t="inlineStr">
+      <c r="D91" s="15" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B90" s="12" t="n"/>
-      <c r="C90" s="22" t="inlineStr">
+      <c r="B92" s="26" t="n"/>
+      <c r="C92" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D90" s="12" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="19" t="inlineStr">
+      <c r="D92" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B91" s="12" t="n"/>
-      <c r="C91" s="22" t="inlineStr">
+      <c r="B93" s="26" t="n"/>
+      <c r="C93" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“You Can Fulfill Challenging Assignments With Jehovah’s Help”: 
 </t>
         </is>
       </c>
-      <c r="D91" s="12" t="n"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="19" t="inlineStr">
+      <c r="D93" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B92" s="12" t="n"/>
-      <c r="C92" s="22" t="inlineStr">
+      <c r="B94" s="26" t="n"/>
+      <c r="C94" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D92" s="12" t="n"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="19" t="inlineStr">
+      <c r="D94" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B93" s="12" t="n"/>
-      <c r="C93" s="22" t="inlineStr">
+      <c r="B95" s="26" t="n"/>
+      <c r="C95" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 7:1-13 (th study 10)
 </t>
         </is>
       </c>
-      <c r="D93" s="12" t="n"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="12" t="n"/>
-      <c r="B94" s="12" t="n"/>
-      <c r="C94" s="12" t="inlineStr"/>
-      <c r="D94" s="12" t="n"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="12" t="n"/>
-      <c r="B95" s="12" t="n"/>
-      <c r="C95" s="23" t="inlineStr">
+      <c r="D95" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="15" t="n"/>
+      <c r="B96" s="15" t="n"/>
+      <c r="C96" s="15" t="inlineStr"/>
+      <c r="D96" s="15" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="15" t="n"/>
+      <c r="B97" s="15" t="n"/>
+      <c r="C97" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D95" s="12" t="n"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="19" t="inlineStr">
+      <c r="D97" s="15" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B96" s="12" t="n"/>
-      <c r="C96" s="22" t="inlineStr">
+      <c r="B98" s="26" t="n"/>
+      <c r="C98" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Leave a jw.org contact card. (th study 16)
 </t>
         </is>
       </c>
-      <c r="D96" s="12" t="n"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="19" t="inlineStr">
+      <c r="D98" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B97" s="12" t="n"/>
-      <c r="C97" s="22" t="inlineStr">
+      <c r="B99" s="26" t="n"/>
+      <c r="C99" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 20)
 </t>
         </is>
       </c>
-      <c r="D97" s="12" t="n"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="19" t="inlineStr">
+      <c r="D99" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B98" s="12" t="n"/>
-      <c r="C98" s="22" t="inlineStr">
+      <c r="B100" s="26" t="n"/>
+      <c r="C100" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w21.06 3-4 ¶3-8 —Theme: Help Your Bible Student to Apply What He Is Learning. (th study 13)
 </t>
         </is>
       </c>
-      <c r="D98" s="12" t="n"/>
-    </row>
-    <row r="99">
-      <c r="A99" s="12" t="n"/>
-      <c r="B99" s="12" t="n"/>
-      <c r="C99" s="12" t="inlineStr"/>
-      <c r="D99" s="12" t="n"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="17" t="inlineStr">
+      <c r="D100" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="15" t="n"/>
+      <c r="B101" s="15" t="n"/>
+      <c r="C101" s="15" t="inlineStr"/>
+      <c r="D101" s="15" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="21" t="inlineStr">
         <is>
           <t>Song 38</t>
         </is>
       </c>
-      <c r="B100" s="12" t="n"/>
-      <c r="C100" s="24" t="inlineStr">
+      <c r="B102" s="15" t="n"/>
+      <c r="C102" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D100" s="12" t="n"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="19" t="inlineStr">
+      <c r="D102" s="15" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="25" t="inlineStr">
         <is>
           <t>(15 min)</t>
         </is>
       </c>
-      <c r="B101" s="12" t="n"/>
-      <c r="C101" s="22" t="inlineStr">
+      <c r="B103" s="26" t="n"/>
+      <c r="C103" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Jehovah Helps Us Through Our Trials”:  Discussion and video.
 </t>
         </is>
       </c>
-      <c r="D101" s="12" t="n"/>
-    </row>
-    <row r="102">
-      <c r="A102" s="19" t="inlineStr">
+      <c r="D103" s="28" t="n">
+        <v>0.30625</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B102" s="12" t="n"/>
-      <c r="C102" s="22" t="inlineStr">
+      <c r="B104" s="26" t="n"/>
+      <c r="C104" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 36
 </t>
         </is>
       </c>
-      <c r="D102" s="12" t="n"/>
-    </row>
-    <row r="103">
-      <c r="A103" s="19" t="inlineStr">
+      <c r="D104" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B103" s="12" t="n"/>
-      <c r="C103" s="22" t="inlineStr">
+      <c r="B105" s="26" t="n"/>
+      <c r="C105" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D103" s="12" t="n"/>
-    </row>
-    <row r="104">
-      <c r="A104" s="12" t="n"/>
-      <c r="B104" s="12" t="n"/>
-      <c r="C104" s="12" t="inlineStr"/>
-      <c r="D104" s="12" t="n"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="17" t="inlineStr">
+      <c r="D105" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="15" t="n"/>
+      <c r="B106" s="15" t="n"/>
+      <c r="C106" s="15" t="inlineStr"/>
+      <c r="D106" s="15" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="21" t="inlineStr">
         <is>
           <t>Song 31</t>
         </is>
       </c>
-      <c r="B105" s="12" t="n"/>
-      <c r="C105" s="18" t="inlineStr">
+      <c r="B107" s="15" t="n"/>
+      <c r="C107" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D105" s="12" t="n"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="12" t="n"/>
-      <c r="B106" s="12" t="n"/>
-      <c r="C106" s="13" t="n"/>
-      <c r="D106" s="12" t="n"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B107" s="15" t="inlineStr">
+      <c r="D107" s="15" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="15" t="n"/>
+      <c r="B108" s="15" t="n"/>
+      <c r="C108" s="31" t="n"/>
+      <c r="D108" s="15" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="17" t="inlineStr">
+        <is>
+          <t>Week 2</t>
+        </is>
+      </c>
+      <c r="B109" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C107" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D107" s="14" t="inlineStr">
+      <c r="C109" s="19" t="inlineStr">
+        <is>
+          <t>1 CHRONICLES 10-12</t>
+        </is>
+      </c>
+      <c r="D109" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" s="17" t="inlineStr">
+    <row r="110">
+      <c r="A110" s="21" t="inlineStr">
         <is>
           <t>Song 94</t>
         </is>
       </c>
-      <c r="B108" s="12" t="n"/>
-      <c r="C108" s="18" t="inlineStr">
+      <c r="B110" s="15" t="n"/>
+      <c r="C110" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D108" s="19" t="inlineStr">
+      <c r="D110" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="12" t="n"/>
-      <c r="B109" s="12" t="n"/>
-      <c r="C109" s="12" t="n"/>
-      <c r="D109" s="20" t="n">
+    <row r="111">
+      <c r="A111" s="15" t="n"/>
+      <c r="B111" s="15" t="n"/>
+      <c r="C111" s="15" t="n"/>
+      <c r="D111" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="12" t="n"/>
-      <c r="B110" s="12" t="n"/>
-      <c r="C110" s="21" t="inlineStr">
+    <row r="112">
+      <c r="A112" s="15" t="n"/>
+      <c r="B112" s="15" t="n"/>
+      <c r="C112" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D110" s="12" t="n"/>
-    </row>
-    <row r="111">
-      <c r="A111" s="19" t="inlineStr">
+      <c r="D112" s="15" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B111" s="12" t="n"/>
-      <c r="C111" s="22" t="inlineStr">
+      <c r="B113" s="26" t="n"/>
+      <c r="C113" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D111" s="12" t="n"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="19" t="inlineStr">
+      <c r="D113" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B112" s="12" t="n"/>
-      <c r="C112" s="22" t="inlineStr">
+      <c r="B114" s="26" t="n"/>
+      <c r="C114" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Strengthen Your Desire to Do God’s Will”: 
 </t>
         </is>
       </c>
-      <c r="D112" s="12" t="n"/>
-    </row>
-    <row r="113">
-      <c r="A113" s="19" t="inlineStr">
+      <c r="D114" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B113" s="12" t="n"/>
-      <c r="C113" s="22" t="inlineStr">
+      <c r="B115" s="26" t="n"/>
+      <c r="C115" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D113" s="12" t="n"/>
-    </row>
-    <row r="114">
-      <c r="A114" s="19" t="inlineStr">
+      <c r="D115" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B114" s="12" t="n"/>
-      <c r="C114" s="22" t="inlineStr">
+      <c r="B116" s="26" t="n"/>
+      <c r="C116" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 11:26-47 (th study 5)
 </t>
         </is>
       </c>
-      <c r="D114" s="12" t="n"/>
-    </row>
-    <row r="115">
-      <c r="A115" s="12" t="n"/>
-      <c r="B115" s="12" t="n"/>
-      <c r="C115" s="12" t="inlineStr"/>
-      <c r="D115" s="12" t="n"/>
-    </row>
-    <row r="116">
-      <c r="A116" s="12" t="n"/>
-      <c r="B116" s="12" t="n"/>
-      <c r="C116" s="23" t="inlineStr">
+      <c r="D116" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="15" t="n"/>
+      <c r="B117" s="15" t="n"/>
+      <c r="C117" s="15" t="inlineStr"/>
+      <c r="D117" s="15" t="n"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="15" t="n"/>
+      <c r="B118" s="15" t="n"/>
+      <c r="C118" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D116" s="12" t="n"/>
-    </row>
-    <row r="117">
-      <c r="A117" s="19" t="inlineStr">
+      <c r="D118" s="15" t="n"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B117" s="12" t="n"/>
-      <c r="C117" s="22" t="inlineStr">
+      <c r="B119" s="26" t="n"/>
+      <c r="C119" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Offer a Bible study. (th study 12)
 </t>
         </is>
       </c>
-      <c r="D117" s="12" t="n"/>
-    </row>
-    <row r="118">
-      <c r="A118" s="19" t="inlineStr">
+      <c r="D119" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B118" s="12" t="n"/>
-      <c r="C118" s="22" t="inlineStr">
+      <c r="B120" s="26" t="n"/>
+      <c r="C120" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video What Happens at a Bible Study? (th study 6)
 </t>
         </is>
       </c>
-      <c r="D118" s="12" t="n"/>
-    </row>
-    <row r="119">
-      <c r="A119" s="19" t="inlineStr">
+      <c r="D120" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B119" s="12" t="n"/>
-      <c r="C119" s="22" t="inlineStr">
+      <c r="B121" s="26" t="n"/>
+      <c r="C121" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Study:  lff lesson 09 intro and points 1-3 (th study 18)
 </t>
         </is>
       </c>
-      <c r="D119" s="12" t="n"/>
-    </row>
-    <row r="120">
-      <c r="A120" s="12" t="n"/>
-      <c r="B120" s="12" t="n"/>
-      <c r="C120" s="12" t="inlineStr"/>
-      <c r="D120" s="12" t="n"/>
-    </row>
-    <row r="121">
-      <c r="A121" s="17" t="inlineStr">
+      <c r="D121" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="15" t="n"/>
+      <c r="B122" s="15" t="n"/>
+      <c r="C122" s="15" t="inlineStr"/>
+      <c r="D122" s="15" t="n"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="21" t="inlineStr">
         <is>
           <t>Song 97</t>
         </is>
       </c>
-      <c r="B121" s="12" t="n"/>
-      <c r="C121" s="24" t="inlineStr">
+      <c r="B123" s="15" t="n"/>
+      <c r="C123" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D121" s="12" t="n"/>
-    </row>
-    <row r="122">
-      <c r="A122" s="19" t="inlineStr">
+      <c r="D123" s="15" t="n"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B122" s="12" t="n"/>
-      <c r="C122" s="22" t="inlineStr">
+      <c r="B124" s="26" t="n"/>
+      <c r="C124" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Search for God’s Thinking”:  Discussion and video.
 </t>
         </is>
       </c>
-      <c r="D122" s="12" t="n"/>
-    </row>
-    <row r="123">
-      <c r="A123" s="19" t="inlineStr">
+      <c r="D124" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B123" s="12" t="n"/>
-      <c r="C123" s="22" t="inlineStr">
+      <c r="B125" s="26" t="n"/>
+      <c r="C125" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Set Goals for the Memorial Season”:  Discussion.
 </t>
         </is>
       </c>
-      <c r="D123" s="12" t="n"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="19" t="inlineStr">
+      <c r="D125" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B124" s="12" t="n"/>
-      <c r="C124" s="22" t="inlineStr">
+      <c r="B126" s="26" t="n"/>
+      <c r="C126" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 points 1-5
 </t>
         </is>
       </c>
-      <c r="D124" s="12" t="n"/>
-    </row>
-    <row r="125">
-      <c r="A125" s="19" t="inlineStr">
+      <c r="D126" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B125" s="12" t="n"/>
-      <c r="C125" s="22" t="inlineStr">
+      <c r="B127" s="26" t="n"/>
+      <c r="C127" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D125" s="12" t="n"/>
-    </row>
-    <row r="126">
-      <c r="A126" s="12" t="n"/>
-      <c r="B126" s="12" t="n"/>
-      <c r="C126" s="12" t="inlineStr"/>
-      <c r="D126" s="12" t="n"/>
-    </row>
-    <row r="127">
-      <c r="A127" s="17" t="inlineStr">
+      <c r="D127" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="15" t="n"/>
+      <c r="B128" s="15" t="n"/>
+      <c r="C128" s="15" t="inlineStr"/>
+      <c r="D128" s="15" t="n"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="21" t="inlineStr">
         <is>
           <t>Song 91</t>
         </is>
       </c>
-      <c r="B127" s="12" t="n"/>
-      <c r="C127" s="18" t="inlineStr">
+      <c r="B129" s="15" t="n"/>
+      <c r="C129" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D127" s="12" t="n"/>
-    </row>
-    <row r="128">
-      <c r="A128" s="12" t="n"/>
-      <c r="B128" s="12" t="n"/>
-      <c r="C128" s="13" t="n"/>
-      <c r="D128" s="12" t="n"/>
-    </row>
-    <row r="129">
-      <c r="A129" s="14" t="inlineStr">
-        <is>
-          <t>[Week]</t>
-        </is>
-      </c>
-      <c r="B129" s="15" t="inlineStr">
+      <c r="D129" s="15" t="n"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="15" t="n"/>
+      <c r="B130" s="15" t="n"/>
+      <c r="C130" s="31" t="n"/>
+      <c r="D130" s="15" t="n"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="17" t="inlineStr">
+        <is>
+          <t>Week 3</t>
+        </is>
+      </c>
+      <c r="B131" s="18" t="inlineStr">
         <is>
           <t>[Date]</t>
         </is>
       </c>
-      <c r="C129" s="16" t="inlineStr">
-        <is>
-          <t>[Scripture]</t>
-        </is>
-      </c>
-      <c r="D129" s="14" t="inlineStr">
+      <c r="C131" s="19" t="inlineStr">
+        <is>
+          <t>1 CHRONICLES 13-16</t>
+        </is>
+      </c>
+      <c r="D131" s="20" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" s="17" t="inlineStr">
+    <row r="132">
+      <c r="A132" s="21" t="inlineStr">
         <is>
           <t>Song 123</t>
         </is>
       </c>
-      <c r="B130" s="12" t="n"/>
-      <c r="C130" s="18" t="inlineStr">
+      <c r="B132" s="15" t="n"/>
+      <c r="C132" s="22" t="inlineStr">
         <is>
           <t>Opening Prayer</t>
         </is>
       </c>
-      <c r="D130" s="19" t="inlineStr">
+      <c r="D132" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">end by </t>
         </is>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="12" t="n"/>
-      <c r="B131" s="12" t="n"/>
-      <c r="C131" s="12" t="n"/>
-      <c r="D131" s="20" t="n">
+    <row r="133">
+      <c r="A133" s="15" t="n"/>
+      <c r="B133" s="15" t="n"/>
+      <c r="C133" s="15" t="n"/>
+      <c r="D133" s="23" t="n">
         <v>0.2958333333333333</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" s="12" t="n"/>
-      <c r="B132" s="12" t="n"/>
-      <c r="C132" s="21" t="inlineStr">
+    <row r="134">
+      <c r="A134" s="15" t="n"/>
+      <c r="B134" s="15" t="n"/>
+      <c r="C134" s="24" t="inlineStr">
         <is>
           <t>Treasures from God's Word</t>
         </is>
       </c>
-      <c r="D132" s="12" t="n"/>
-    </row>
-    <row r="133">
-      <c r="A133" s="19" t="inlineStr">
+      <c r="D134" s="15" t="n"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="25" t="inlineStr">
         <is>
           <t>(1 min)</t>
         </is>
       </c>
-      <c r="B133" s="12" t="n"/>
-      <c r="C133" s="22" t="inlineStr">
+      <c r="B135" s="26" t="n"/>
+      <c r="C135" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Opening Comments 
 </t>
         </is>
       </c>
-      <c r="D133" s="12" t="n"/>
-    </row>
-    <row r="134">
-      <c r="A134" s="19" t="inlineStr">
+      <c r="D135" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B134" s="12" t="n"/>
-      <c r="C134" s="22" t="inlineStr">
+      <c r="B136" s="26" t="n"/>
+      <c r="C136" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">“Following Direction Leads to Success”: 
 </t>
         </is>
       </c>
-      <c r="D134" s="12" t="n"/>
-    </row>
-    <row r="135">
-      <c r="A135" s="19" t="inlineStr">
+      <c r="D136" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="25" t="inlineStr">
         <is>
           <t>(10 min)</t>
         </is>
       </c>
-      <c r="B135" s="12" t="n"/>
-      <c r="C135" s="22" t="inlineStr">
+      <c r="B137" s="26" t="n"/>
+      <c r="C137" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Spiritual Gems: 
 </t>
         </is>
       </c>
-      <c r="D135" s="12" t="n"/>
-    </row>
-    <row r="136">
-      <c r="A136" s="19" t="inlineStr">
+      <c r="D137" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B136" s="12" t="n"/>
-      <c r="C136" s="22" t="inlineStr">
+      <c r="B138" s="26" t="n"/>
+      <c r="C138" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Bible Reading:  1Ch 13:1-14 (th study 11)
 </t>
         </is>
       </c>
-      <c r="D136" s="12" t="n"/>
-    </row>
-    <row r="137">
-      <c r="A137" s="12" t="n"/>
-      <c r="B137" s="12" t="n"/>
-      <c r="C137" s="12" t="inlineStr"/>
-      <c r="D137" s="12" t="n"/>
-    </row>
-    <row r="138">
-      <c r="A138" s="12" t="n"/>
-      <c r="B138" s="12" t="n"/>
-      <c r="C138" s="23" t="inlineStr">
+      <c r="D138" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="15" t="n"/>
+      <c r="B139" s="15" t="n"/>
+      <c r="C139" s="15" t="inlineStr"/>
+      <c r="D139" s="15" t="n"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="15" t="n"/>
+      <c r="B140" s="15" t="n"/>
+      <c r="C140" s="29" t="inlineStr">
         <is>
           <t>Apply Yourself to the Field Ministry</t>
         </is>
       </c>
-      <c r="D138" s="12" t="n"/>
-    </row>
-    <row r="139">
-      <c r="A139" s="19" t="inlineStr">
+      <c r="D140" s="15" t="n"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B139" s="12" t="n"/>
-      <c r="C139" s="22" t="inlineStr">
+      <c r="B141" s="26" t="n"/>
+      <c r="C141" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Respond to a common objection. (th study 18)
 </t>
         </is>
       </c>
-      <c r="D139" s="12" t="n"/>
-    </row>
-    <row r="140">
-      <c r="A140" s="19" t="inlineStr">
+      <c r="D141" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="25" t="inlineStr">
         <is>
           <t>(4 min)</t>
         </is>
       </c>
-      <c r="B140" s="12" t="n"/>
-      <c r="C140" s="22" t="inlineStr">
+      <c r="B142" s="26" t="n"/>
+      <c r="C142" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 7)
 </t>
         </is>
       </c>
-      <c r="D140" s="12" t="n"/>
-    </row>
-    <row r="141">
-      <c r="A141" s="19" t="inlineStr">
+      <c r="D142" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B141" s="12" t="n"/>
-      <c r="C141" s="22" t="inlineStr">
+      <c r="B143" s="26" t="n"/>
+      <c r="C143" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Talk:  w16.01 13-14 ¶7-10 —Theme: “The Love the Christ Has Compels Us.” —2Co 5:14. (th study 8)
 </t>
         </is>
       </c>
-      <c r="D141" s="12" t="n"/>
-    </row>
-    <row r="142">
-      <c r="A142" s="12" t="n"/>
-      <c r="B142" s="12" t="n"/>
-      <c r="C142" s="12" t="inlineStr"/>
-      <c r="D142" s="12" t="n"/>
-    </row>
-    <row r="143">
-      <c r="A143" s="17" t="inlineStr">
+      <c r="D143" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="15" t="n"/>
+      <c r="B144" s="15" t="n"/>
+      <c r="C144" s="15" t="inlineStr"/>
+      <c r="D144" s="15" t="n"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="21" t="inlineStr">
         <is>
           <t>Song 86</t>
         </is>
       </c>
-      <c r="B143" s="12" t="n"/>
-      <c r="C143" s="24" t="inlineStr">
+      <c r="B145" s="15" t="n"/>
+      <c r="C145" s="30" t="inlineStr">
         <is>
           <t>Living as Christians</t>
         </is>
       </c>
-      <c r="D143" s="12" t="n"/>
-    </row>
-    <row r="144">
-      <c r="A144" s="19" t="inlineStr">
+      <c r="D145" s="15" t="n"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B144" s="12" t="n"/>
-      <c r="C144" s="22" t="inlineStr">
+      <c r="B146" s="26" t="n"/>
+      <c r="C146" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Become Jehovah’s Friend —Pay Attention at the Meetings:  Discussion. Play the video. Then, if possible, ask selected children: Why should we pay attention at meetings? What can help you to do so?
 </t>
         </is>
       </c>
-      <c r="D144" s="12" t="n"/>
-    </row>
-    <row r="145">
-      <c r="A145" s="19" t="inlineStr">
+      <c r="D146" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="25" t="inlineStr">
         <is>
           <t>(5 min)</t>
         </is>
       </c>
-      <c r="B145" s="12" t="n"/>
-      <c r="C145" s="22" t="inlineStr">
+      <c r="B147" s="26" t="n"/>
+      <c r="C147" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Local Needs: 
 </t>
         </is>
       </c>
-      <c r="D145" s="12" t="n"/>
-    </row>
-    <row r="146">
-      <c r="A146" s="19" t="inlineStr">
+      <c r="D147" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="25" t="inlineStr">
         <is>
           <t>(30 min)</t>
         </is>
       </c>
-      <c r="B146" s="12" t="n"/>
-      <c r="C146" s="22" t="inlineStr">
+      <c r="B148" s="26" t="n"/>
+      <c r="C148" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Congregation Bible Study:  lff lesson 37 point 6 and summary, review, and goal
 </t>
         </is>
       </c>
-      <c r="D146" s="12" t="n"/>
-    </row>
-    <row r="147">
-      <c r="A147" s="19" t="inlineStr">
+      <c r="D148" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="25" t="inlineStr">
         <is>
           <t>(3 min)</t>
         </is>
       </c>
-      <c r="B147" s="12" t="n"/>
-      <c r="C147" s="22" t="inlineStr">
+      <c r="B149" s="26" t="n"/>
+      <c r="C149" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">Concluding Comments 
 </t>
         </is>
       </c>
-      <c r="D147" s="12" t="n"/>
-    </row>
-    <row r="148">
-      <c r="A148" s="12" t="n"/>
-      <c r="B148" s="12" t="n"/>
-      <c r="C148" s="12" t="inlineStr"/>
-      <c r="D148" s="12" t="n"/>
-    </row>
-    <row r="149">
-      <c r="A149" s="17" t="inlineStr">
+      <c r="D149" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="15" t="n"/>
+      <c r="B150" s="15" t="n"/>
+      <c r="C150" s="15" t="inlineStr"/>
+      <c r="D150" s="15" t="n"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="21" t="inlineStr">
         <is>
           <t>Song 21</t>
         </is>
       </c>
-      <c r="B149" s="12" t="n"/>
-      <c r="C149" s="18" t="inlineStr">
+      <c r="B151" s="15" t="n"/>
+      <c r="C151" s="22" t="inlineStr">
         <is>
           <t>Closing Prayer</t>
         </is>
       </c>
-      <c r="D149" s="12" t="n"/>
-    </row>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
+      <c r="D151" s="15" t="n"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="17" t="inlineStr">
+        <is>
+          <t>Week 4</t>
+        </is>
+      </c>
+      <c r="B152" s="18" t="inlineStr">
+        <is>
+          <t>[Date]</t>
+        </is>
+      </c>
+      <c r="C152" s="19" t="inlineStr">
+        <is>
+          <t>1 CHRONICLES 17-19</t>
+        </is>
+      </c>
+      <c r="D152" s="20" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="21" t="inlineStr">
+        <is>
+          <t>Song 110</t>
+        </is>
+      </c>
+      <c r="B153" s="15" t="n"/>
+      <c r="C153" s="22" t="inlineStr">
+        <is>
+          <t>Opening Prayer</t>
+        </is>
+      </c>
+      <c r="D153" s="23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">end by </t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="15" t="n"/>
+      <c r="B154" s="15" t="n"/>
+      <c r="C154" s="15" t="n"/>
+      <c r="D154" s="23" t="n">
+        <v>0.2958333333333333</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="15" t="n"/>
+      <c r="B155" s="15" t="n"/>
+      <c r="C155" s="24" t="inlineStr">
+        <is>
+          <t>Treasures from God's Word</t>
+        </is>
+      </c>
+      <c r="D155" s="15" t="n"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="25" t="inlineStr">
+        <is>
+          <t>(1 min)</t>
+        </is>
+      </c>
+      <c r="B156" s="26" t="n"/>
+      <c r="C156" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opening Comments 
+</t>
+        </is>
+      </c>
+      <c r="D156" s="28" t="n">
+        <v>0.2965277777777778</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="25" t="inlineStr">
+        <is>
+          <t>(10 min)</t>
+        </is>
+      </c>
+      <c r="B157" s="26" t="n"/>
+      <c r="C157" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Maintain Your Joy Despite Disappointments”: 
+</t>
+        </is>
+      </c>
+      <c r="D157" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="25" t="inlineStr">
+        <is>
+          <t>(10 min)</t>
+        </is>
+      </c>
+      <c r="B158" s="26" t="n"/>
+      <c r="C158" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spiritual Gems: 
+</t>
+        </is>
+      </c>
+      <c r="D158" s="28" t="n">
+        <v>0.3027777777777778</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="25" t="inlineStr">
+        <is>
+          <t>(4 min)</t>
+        </is>
+      </c>
+      <c r="B159" s="26" t="n"/>
+      <c r="C159" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bible Reading:  1Ch 18:1-17 (th study 2)
+</t>
+        </is>
+      </c>
+      <c r="D159" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="15" t="n"/>
+      <c r="B160" s="15" t="n"/>
+      <c r="C160" s="15" t="inlineStr"/>
+      <c r="D160" s="15" t="n"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="15" t="n"/>
+      <c r="B161" s="15" t="n"/>
+      <c r="C161" s="29" t="inlineStr">
+        <is>
+          <t>Apply Yourself to the Field Ministry</t>
+        </is>
+      </c>
+      <c r="D161" s="15" t="n"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="25" t="inlineStr">
+        <is>
+          <t>(3 min)</t>
+        </is>
+      </c>
+      <c r="B162" s="26" t="n"/>
+      <c r="C162" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Initial Call:  Begin with the sample conversation topic. Introduce and discuss (but do not play) the video Jehovah’s Witnesses —Who Are We? (th study 17)
+</t>
+        </is>
+      </c>
+      <c r="D162" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="25" t="inlineStr">
+        <is>
+          <t>(4 min)</t>
+        </is>
+      </c>
+      <c r="B163" s="26" t="n"/>
+      <c r="C163" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Return Visit:  Begin with the sample conversation topic. Offer a publication from the Teaching Toolbox. (th study 3)
+</t>
+        </is>
+      </c>
+      <c r="D163" s="28" t="n">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="25" t="inlineStr">
+        <is>
+          <t>(5 min)</t>
+        </is>
+      </c>
+      <c r="B164" s="26" t="n"/>
+      <c r="C164" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bible Study:  lff lesson 09 point 4 (th study 9)
+</t>
+        </is>
+      </c>
+      <c r="D164" s="28" t="n">
+        <v>0.2993055555555555</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="15" t="n"/>
+      <c r="B165" s="15" t="n"/>
+      <c r="C165" s="15" t="inlineStr"/>
+      <c r="D165" s="15" t="n"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="21" t="inlineStr">
+        <is>
+          <t>Song 64</t>
+        </is>
+      </c>
+      <c r="B166" s="15" t="n"/>
+      <c r="C166" s="30" t="inlineStr">
+        <is>
+          <t>Living as Christians</t>
+        </is>
+      </c>
+      <c r="D166" s="15" t="n"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="25" t="inlineStr">
+        <is>
+          <t>(15 min)</t>
+        </is>
+      </c>
+      <c r="B167" s="26" t="n"/>
+      <c r="C167" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Annual Service Report:  Discussion. After reading the announcement from the branch office regarding the annual service report, invite the audience to highlight other positive aspects of the 2022 Service Year Report of Jehovah’s Witnesses Worldwide. Interview publishers, selected in advance, who had encouraging experiences in the ministry during the past year.
+</t>
+        </is>
+      </c>
+      <c r="D167" s="28" t="n">
+        <v>0.30625</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="25" t="inlineStr">
+        <is>
+          <t>(30 min)</t>
+        </is>
+      </c>
+      <c r="B168" s="26" t="n"/>
+      <c r="C168" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Congregation Bible Study:  lff lesson 38 points 1-4
+</t>
+        </is>
+      </c>
+      <c r="D168" s="28" t="n">
+        <v>0.3166666666666667</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="25" t="inlineStr">
+        <is>
+          <t>(3 min)</t>
+        </is>
+      </c>
+      <c r="B169" s="26" t="n"/>
+      <c r="C169" s="27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concluding Comments 
+</t>
+        </is>
+      </c>
+      <c r="D169" s="28" t="n">
+        <v>0.2979166666666667</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="15" t="n"/>
+      <c r="B170" s="15" t="n"/>
+      <c r="C170" s="15" t="inlineStr"/>
+      <c r="D170" s="15" t="n"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="21" t="inlineStr">
+        <is>
+          <t>Song 141</t>
+        </is>
+      </c>
+      <c r="B171" s="15" t="n"/>
+      <c r="C171" s="22" t="inlineStr">
+        <is>
+          <t>Closing Prayer</t>
+        </is>
+      </c>
+      <c r="D171" s="15" t="n"/>
+    </row>
     <row r="172"/>
     <row r="173"/>
     <row r="174"/>
@@ -3350,6 +3824,11 @@
     <row r="998"/>
     <row r="999"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B47:C47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>